<commit_message>
Modified SPL parser to (1) include MarketingStatus and ApprovalAppId for products with parts and (2) expand ALLERGENIC products selection. Added modified SPL files. Added new Rancho dump. Added new GSRS dump. Removed old files. Modified loading scripts accordingly.
</commit_message>
<xml_diff>
--- a/data/dev_status_logic.xlsx
+++ b/data/dev_status_logic.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\stitcher\data\"/>
@@ -15,14 +15,14 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$D$124</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="85">
   <si>
     <t>MarketingStatus</t>
   </si>
@@ -60,21 +60,36 @@
     <t>UNAPPROVED DRUG OTHER</t>
   </si>
   <si>
+    <t>OTC monograph final</t>
+  </si>
+  <si>
     <t>MEDICAL DEVICE</t>
   </si>
   <si>
+    <t>US Approved OTC</t>
+  </si>
+  <si>
+    <t>OTC monograph not final</t>
+  </si>
+  <si>
+    <t>NDA</t>
+  </si>
+  <si>
+    <t>ANDA</t>
+  </si>
+  <si>
+    <t>unapproved drug other</t>
+  </si>
+  <si>
+    <t>PLASMA DERIVATIVE</t>
+  </si>
+  <si>
+    <t>Exempt device</t>
+  </si>
+  <si>
     <t>Other</t>
   </si>
   <si>
-    <t>PLASMA DERIVATIVE</t>
-  </si>
-  <si>
-    <t>ANDA</t>
-  </si>
-  <si>
-    <t>Exempt device</t>
-  </si>
-  <si>
     <t>CELLULAR THERAPY</t>
   </si>
   <si>
@@ -111,12 +126,6 @@
     <t>Medical Food</t>
   </si>
   <si>
-    <t>OTC monograph final</t>
-  </si>
-  <si>
-    <t>US Approved OTC</t>
-  </si>
-  <si>
     <t>premarket notification</t>
   </si>
   <si>
@@ -126,9 +135,6 @@
     <t>PRESCRIPTION MEDICAL DEVICE LABEL</t>
   </si>
   <si>
-    <t>OTC monograph not final</t>
-  </si>
-  <si>
     <t>exempt device</t>
   </si>
   <si>
@@ -141,12 +147,12 @@
     <t>EXEMPT DEVICE</t>
   </si>
   <si>
-    <t>unapproved drug other</t>
-  </si>
-  <si>
     <t>HUMAN COMPOUNDED DRUG LABEL</t>
   </si>
   <si>
+    <t>PREMARKET NOTIFICATION</t>
+  </si>
+  <si>
     <t>EXPORT ONLY</t>
   </si>
   <si>
@@ -168,15 +174,15 @@
     <t>RECOMBINANT DEOXYRIBONUCLEIC ACID CONSTRUCT LABEL</t>
   </si>
   <si>
-    <t>PREMARKET NOTIFICATION</t>
-  </si>
-  <si>
     <t>export only</t>
   </si>
   <si>
     <t>Cosmetic</t>
   </si>
   <si>
+    <t>Unapproved drug for use in drug shortage</t>
+  </si>
+  <si>
     <t>Manufactures Non-Generics</t>
   </si>
   <si>
@@ -186,15 +192,15 @@
     <t>BULK INGREDIENT - ANIMAL DRUG</t>
   </si>
   <si>
+    <t>Premarket Application</t>
+  </si>
+  <si>
     <t>HUMAN PRESCRIPTION DRUG LABEL</t>
   </si>
   <si>
     <t>HUMAN PRESCRIPTION DRUG LABEL WITH HIGHLIGHTS</t>
   </si>
   <si>
-    <t>NDA</t>
-  </si>
-  <si>
     <t>NDA authorized generic</t>
   </si>
   <si>
@@ -226,9 +232,6 @@
   </si>
   <si>
     <t>NDA AUTHORIZED GENERIC</t>
-  </si>
-  <si>
-    <t>Unapproved drug for use in drug shortage</t>
   </si>
   <si>
     <t>OTC MONOGRAPH FINAL</t>
@@ -616,12 +619,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,72 +692,72 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -763,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -774,16 +776,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -791,32 +793,32 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -825,133 +827,133 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -959,49 +961,49 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -1012,66 +1014,66 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -1082,44 +1084,44 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1127,7 +1129,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -1138,10 +1140,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -1152,63 +1154,63 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
@@ -1222,10 +1224,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -1236,10 +1238,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -1250,128 +1252,128 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1379,7 +1381,7 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -1390,10 +1392,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
@@ -1407,7 +1409,7 @@
         <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
@@ -1421,7 +1423,7 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
         <v>9</v>
@@ -1432,10 +1434,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
@@ -1446,10 +1448,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
@@ -1460,10 +1462,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
@@ -1474,10 +1476,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
@@ -1488,10 +1490,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
@@ -1502,80 +1504,80 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
@@ -1586,10 +1588,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
@@ -1600,10 +1602,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
@@ -1614,10 +1616,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
@@ -1628,52 +1630,52 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
       </c>
       <c r="D73" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B74" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B75" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
@@ -1684,108 +1686,108 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B76" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B77" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B78" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B79" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B80" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B81" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B82" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B83" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
@@ -1799,111 +1801,111 @@
         <v>71</v>
       </c>
       <c r="B84" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B85" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C86" t="s">
         <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C87" t="s">
         <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="B88" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C88" t="s">
         <v>6</v>
       </c>
       <c r="D88" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="B89" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C89" t="s">
         <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B90" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B91" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C91" t="s">
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -1911,77 +1913,77 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C92" t="s">
         <v>6</v>
       </c>
       <c r="D92" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="B94" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C94" t="s">
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="B95" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C95" t="s">
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B96" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B97" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
@@ -1992,24 +1994,24 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B98" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C98" t="s">
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B99" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C99" t="s">
         <v>6</v>
@@ -2020,24 +2022,24 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="B100" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C100" t="s">
         <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="B101" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C101" t="s">
         <v>6</v>
@@ -2048,38 +2050,38 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B102" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C102" t="s">
         <v>6</v>
       </c>
       <c r="D102" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B103" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C103" t="s">
         <v>6</v>
       </c>
       <c r="D103" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
@@ -2090,38 +2092,38 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B105" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C105" t="s">
         <v>6</v>
       </c>
       <c r="D105" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B106" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C106" t="s">
         <v>6</v>
       </c>
       <c r="D106" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B107" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C107" t="s">
         <v>6</v>
@@ -2132,44 +2134,44 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B108" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B109" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C109" t="s">
         <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B110" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C110" t="s">
         <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2177,129 +2179,199 @@
         <v>81</v>
       </c>
       <c r="B111" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B112" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C112" t="s">
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="B113" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B114" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C114" t="s">
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B115" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C115" t="s">
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="B116" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C116" t="s">
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B117" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C117" t="s">
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B119" t="s">
+        <v>76</v>
+      </c>
+      <c r="C119" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>37</v>
+      </c>
+      <c r="B120" t="s">
+        <v>76</v>
+      </c>
+      <c r="C120" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>59</v>
+      </c>
+      <c r="B121" t="s">
+        <v>76</v>
+      </c>
+      <c r="C121" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>69</v>
+      </c>
+      <c r="B122" t="s">
+        <v>76</v>
+      </c>
+      <c r="C122" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>75</v>
       </c>
-      <c r="C119" t="s">
-        <v>6</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="B123" t="s">
+        <v>76</v>
+      </c>
+      <c r="C123" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>74</v>
+      </c>
+      <c r="B124" t="s">
+        <v>76</v>
+      </c>
+      <c r="C124" t="s">
+        <v>6</v>
+      </c>
+      <c r="D124" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D124"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
handle allergenic extracts better:
</commit_message>
<xml_diff>
--- a/data/dev_status_logic.xlsx
+++ b/data/dev_status_logic.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\RB\NCATS\2017-06-09 drug pages\2018-09-24 dev status logic update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/southalln/git/stitcher/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B018485A-12C4-634C-B9C4-09097EAE647C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18520" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="90">
   <si>
     <t>MarketingStatus</t>
   </si>
@@ -289,12 +290,15 @@
   </si>
   <si>
     <t>Unapproved homeopathic</t>
+  </si>
+  <si>
+    <t>US Approved Allergenic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,25 +634,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44.33203125" customWidth="1"/>
-    <col min="2" max="2" width="52.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -688,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -702,13 +706,13 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -728,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -748,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -768,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -788,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -808,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -828,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -848,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -868,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -888,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -908,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -928,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -948,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -968,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -988,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1028,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1068,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1108,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1128,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1148,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1168,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1188,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1208,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1228,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1248,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1268,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1282,13 +1286,13 @@
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -1308,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1322,13 +1326,13 @@
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1348,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1368,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1388,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1408,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1422,13 +1426,13 @@
         <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1468,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1508,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -1528,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1548,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -1588,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1608,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1628,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1648,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1668,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1708,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -1748,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1768,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1782,13 +1786,13 @@
         <v>63</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -1808,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -1828,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -1848,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -1868,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -1888,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1908,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -1948,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -1988,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>21</v>
       </c>
@@ -2008,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -2028,7 +2032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -2068,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -2088,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -2108,7 +2112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -2128,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -2148,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -2188,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>35</v>
       </c>
@@ -2208,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>73</v>
       </c>
@@ -2228,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>74</v>
       </c>
@@ -2248,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>49</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>37</v>
       </c>
@@ -2288,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>30</v>
       </c>
@@ -2308,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>31</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -2348,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>75</v>
       </c>
@@ -2368,7 +2372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>76</v>
       </c>
@@ -2388,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>41</v>
       </c>
@@ -2408,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -2428,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>78</v>
       </c>
@@ -2448,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>79</v>
       </c>
@@ -2468,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -2488,7 +2492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>59</v>
       </c>
@@ -2508,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>18</v>
       </c>
@@ -2528,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -2548,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>20</v>
       </c>
@@ -2568,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>74</v>
       </c>
@@ -2588,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>67</v>
       </c>
@@ -2608,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>69</v>
       </c>
@@ -2628,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>58</v>
       </c>
@@ -2648,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>19</v>
       </c>
@@ -2668,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>21</v>
       </c>
@@ -2688,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>42</v>
       </c>
@@ -2708,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>65</v>
       </c>
@@ -2728,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>82</v>
       </c>
@@ -2748,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>83</v>
       </c>
@@ -2768,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>84</v>
       </c>
@@ -2788,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>85</v>
       </c>
@@ -2808,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>14</v>
       </c>
@@ -2828,7 +2832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -2848,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>86</v>
       </c>
@@ -2868,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>41</v>
       </c>
@@ -2888,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>76</v>
       </c>
@@ -2908,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>87</v>
       </c>
@@ -2928,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>88</v>
       </c>
@@ -2948,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>79</v>
       </c>
@@ -2968,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>59</v>
       </c>
@@ -2989,7 +2993,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>